<commit_message>
2. ConsentPageTest, GreatNewsPageTest, NameDetailsPageTest, GreetingPageTest are completed. ProgramsInfPageTest is in progress.
</commit_message>
<xml_diff>
--- a/Excels/SimpleTherapy_Details.xlsx
+++ b/Excels/SimpleTherapy_Details.xlsx
@@ -5,16 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snehal-Vinayak\IdeaProjects\SimpleTherapy_Web_Automation\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snehal-Vinayak\IdeaProjects\SimpleTherapy_Automation\SimpleTherapy_Web_Automation\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B20B35-DC9B-47F4-B4DB-EE262CC62177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3756CB75-EE9D-44CE-969B-8A76794E1E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{4838E644-DBD1-4BD5-84C0-B33ABF6093BA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="5" xr2:uid="{4838E644-DBD1-4BD5-84C0-B33ABF6093BA}"/>
   </bookViews>
   <sheets>
     <sheet name="LandingPage_Data" sheetId="1" r:id="rId1"/>
-    <sheet name="RegistrationPage_Data" sheetId="2" r:id="rId2"/>
+    <sheet name="ConsentPage_Data" sheetId="3" r:id="rId2"/>
+    <sheet name="GreatNewsPage_Data" sheetId="2" r:id="rId3"/>
+    <sheet name="NameDetailsPage_Data" sheetId="4" r:id="rId4"/>
+    <sheet name="GreetingPage_Data" sheetId="5" r:id="rId5"/>
+    <sheet name="ProgramsInfoPage_Data" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>TitleHeading</t>
   </si>
@@ -85,6 +89,42 @@
   </si>
   <si>
     <t>GreatNewsHeading</t>
+  </si>
+  <si>
+    <t>What is your legal first and last name?</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>Sagar</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Pangale</t>
+  </si>
+  <si>
+    <t>PrefName</t>
+  </si>
+  <si>
+    <t>Sag</t>
+  </si>
+  <si>
+    <t>NameDetailsHeading</t>
+  </si>
+  <si>
+    <t>GreetingHeading</t>
+  </si>
+  <si>
+    <t>Nice to meet you, Sag!</t>
+  </si>
+  <si>
+    <t>ProgramsInfoHeading</t>
+  </si>
+  <si>
+    <t>Care made simple</t>
   </si>
 </sst>
 </file>
@@ -156,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -181,6 +221,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,7 +561,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -579,39 +622,68 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819201CF-8B1E-4859-A8E6-42C06185CA87}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3395EEC3-F750-48BC-9356-FE0636C56AD8}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819201CF-8B1E-4859-A8E6-42C06185CA87}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.90625" customWidth="1"/>
     <col min="2" max="2" width="16.6328125" customWidth="1"/>
     <col min="3" max="3" width="24.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -619,4 +691,173 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F461D54-812F-4A6E-AE95-2C6105739A09}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14" style="10" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="11.08984375" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55BF6945-9FFC-4C1A-B356-633FD7C623EB}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.6328125" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1C3BB4-F0EC-4827-AF9D-78A937D03CAB}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="21.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
3. RegistrationFlowTest is in progress.
</commit_message>
<xml_diff>
--- a/Excels/SimpleTherapy_Details.xlsx
+++ b/Excels/SimpleTherapy_Details.xlsx
@@ -1,24 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snehal-Vinayak\IdeaProjects\SimpleTherapy_Automation\SimpleTherapy_Web_Automation\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3756CB75-EE9D-44CE-969B-8A76794E1E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366B66D8-1E38-46B4-8F72-2DB67757EADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="5" xr2:uid="{4838E644-DBD1-4BD5-84C0-B33ABF6093BA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4838E644-DBD1-4BD5-84C0-B33ABF6093BA}"/>
   </bookViews>
   <sheets>
-    <sheet name="LandingPage_Data" sheetId="1" r:id="rId1"/>
-    <sheet name="ConsentPage_Data" sheetId="3" r:id="rId2"/>
-    <sheet name="GreatNewsPage_Data" sheetId="2" r:id="rId3"/>
-    <sheet name="NameDetailsPage_Data" sheetId="4" r:id="rId4"/>
-    <sheet name="GreetingPage_Data" sheetId="5" r:id="rId5"/>
-    <sheet name="ProgramsInfoPage_Data" sheetId="6" r:id="rId6"/>
+    <sheet name="Dev2" sheetId="7" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>TitleHeading</t>
   </si>
@@ -52,30 +47,12 @@
     <t>Need Help? Call us at</t>
   </si>
   <si>
-    <t>PopupHeading</t>
-  </si>
-  <si>
     <t>EmployerName</t>
   </si>
   <si>
     <t>dev2</t>
   </si>
   <si>
-    <t>OperatorHeading</t>
-  </si>
-  <si>
-    <t>PolishLanguageTitleHeading</t>
-  </si>
-  <si>
-    <t>Witamy w SimpleTherapy</t>
-  </si>
-  <si>
-    <t>ExpectedLanguageCode</t>
-  </si>
-  <si>
-    <t>pl</t>
-  </si>
-  <si>
     <t>We're here to answer your questions about SimpleTherapy. Ask us anything.</t>
   </si>
   <si>
@@ -115,16 +92,22 @@
     <t>NameDetailsHeading</t>
   </si>
   <si>
-    <t>GreetingHeading</t>
-  </si>
-  <si>
     <t>Nice to meet you, Sag!</t>
   </si>
   <si>
-    <t>ProgramsInfoHeading</t>
-  </si>
-  <si>
     <t>Care made simple</t>
+  </si>
+  <si>
+    <t>ChatBotHeading</t>
+  </si>
+  <si>
+    <t>NeedHelpPopupHeading</t>
+  </si>
+  <si>
+    <t>FirstGreetingHeading</t>
+  </si>
+  <si>
+    <t>SecondGreetingHeading</t>
   </si>
 </sst>
 </file>
@@ -196,22 +179,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -219,8 +193,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -557,304 +529,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{820E04B9-9C88-4D92-980D-50F0FD5F9AA5}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C8AB82-C9FB-4A1D-8D28-EAF73CBFCFBA}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="24.7265625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.54296875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="11.1796875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="21.26953125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="18.453125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="9.6328125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="10" style="5" customWidth="1"/>
+    <col min="11" max="11" width="19.08984375" style="5" customWidth="1"/>
+    <col min="12" max="12" width="20.90625" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:12" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3395EEC3-F750-48BC-9356-FE0636C56AD8}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="2" max="2" width="17.36328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819201CF-8B1E-4859-A8E6-42C06185CA87}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="16.90625" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
-    <col min="3" max="3" width="24.90625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="I2" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F461D54-812F-4A6E-AE95-2C6105739A09}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14" style="10" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="9.6328125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="11.08984375" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="J2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55BF6945-9FFC-4C1A-B356-633FD7C623EB}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13.6328125" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" customWidth="1"/>
-    <col min="3" max="3" width="9.54296875" customWidth="1"/>
-    <col min="4" max="4" width="10.6328125" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1C3BB4-F0EC-4827-AF9D-78A937D03CAB}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14.08984375" customWidth="1"/>
-    <col min="2" max="2" width="11.26953125" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="21.08984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3. RegistrationFlowTest and DashboardPageTest is completed and ProfileDetailsPageTest is in progress.
</commit_message>
<xml_diff>
--- a/Excels/SimpleTherapy_Details.xlsx
+++ b/Excels/SimpleTherapy_Details.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snehal-Vinayak\IdeaProjects\SimpleTherapy_Automation\SimpleTherapy_Web_Automation\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366B66D8-1E38-46B4-8F72-2DB67757EADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A353AF01-001D-4739-A126-F36DD0EB5EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4838E644-DBD1-4BD5-84C0-B33ABF6093BA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{4838E644-DBD1-4BD5-84C0-B33ABF6093BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Dev2" sheetId="7" r:id="rId1"/>
+    <sheet name="OTP_Data" sheetId="8" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
   <si>
     <t>TitleHeading</t>
   </si>
@@ -108,6 +109,132 @@
   </si>
   <si>
     <t>SecondGreetingHeading</t>
+  </si>
+  <si>
+    <t>ThirdGreetingHeading</t>
+  </si>
+  <si>
+    <t>Personal, 1-on-1</t>
+  </si>
+  <si>
+    <t>Tell us about yourself</t>
+  </si>
+  <si>
+    <t>PersonalInfoHeading</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>ZipCode</t>
+  </si>
+  <si>
+    <t>Fremont</t>
+  </si>
+  <si>
+    <t>Provide your location</t>
+  </si>
+  <si>
+    <t>AddressHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 440 555 5555</t>
+  </si>
+  <si>
+    <t>1950, San benito dr</t>
+  </si>
+  <si>
+    <t>ActivationCodeHeading</t>
+  </si>
+  <si>
+    <t>Activation Code</t>
+  </si>
+  <si>
+    <t>ActivationCode</t>
+  </si>
+  <si>
+    <t>ST10200</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Sagar@1234</t>
+  </si>
+  <si>
+    <t>SignUpPasswordHeading</t>
+  </si>
+  <si>
+    <t>Create Your Account</t>
+  </si>
+  <si>
+    <t>AccountSecurityHeading</t>
+  </si>
+  <si>
+    <t>Keep Your Account Safe</t>
+  </si>
+  <si>
+    <t>AccountSecurityOtpHeading</t>
+  </si>
+  <si>
+    <t>Secure Your Account</t>
+  </si>
+  <si>
+    <t>PostAuthHeading</t>
+  </si>
+  <si>
+    <t>Your account is activated</t>
+  </si>
+  <si>
+    <t>Env</t>
+  </si>
+  <si>
+    <t>Dev2</t>
+  </si>
+  <si>
+    <t>OtpSecret</t>
+  </si>
+  <si>
+    <t>What brings you here today?</t>
+  </si>
+  <si>
+    <t>BenefitCardHeading</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>ProfileDetailsHeading</t>
+  </si>
+  <si>
+    <t>Profile Details</t>
+  </si>
+  <si>
+    <t>sagar+202601133@mobiuso.com</t>
+  </si>
+  <si>
+    <t>KJTDCYSPMUQVISZKOBHVGQRFOBFCMUDJ</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>California</t>
   </si>
 </sst>
 </file>
@@ -152,7 +279,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -175,11 +302,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -196,6 +336,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,30 +688,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C8AB82-C9FB-4A1D-8D28-EAF73CBFCFBA}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="21.26953125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="17.81640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="18.453125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="9.6328125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="10" style="5" customWidth="1"/>
-    <col min="11" max="11" width="19.08984375" style="5" customWidth="1"/>
-    <col min="12" max="12" width="20.90625" style="5" customWidth="1"/>
-    <col min="13" max="16384" width="8.7265625" style="5"/>
+    <col min="1" max="1" width="15" style="5" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.453125" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.81640625" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.26953125" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.81640625" style="5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.81640625" style="5" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.36328125" style="5" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.81640625" style="5" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.6328125" style="5" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10" style="5" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.54296875" style="5" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="22.36328125" style="5" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="20.90625" style="5" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.90625" style="5" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.7265625" style="5" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="18.54296875" style="5" customWidth="1" collapsed="1"/>
+    <col min="17" max="19" width="8.7265625" style="5" collapsed="1"/>
+    <col min="20" max="20" width="21.453125" style="5" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="14.7265625" style="5" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="21.7265625" style="5" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.7265625" style="5" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="21.6328125" style="5" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="25.54296875" style="5" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="15.54296875" style="5" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="18.7265625" style="5" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="19.81640625" style="5" customWidth="1" collapsed="1"/>
+    <col min="29" max="16384" width="8.7265625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -590,8 +762,56 @@
       <c r="L1" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="M1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -622,11 +842,164 @@
       <c r="J2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="8" t="s">
         <v>18</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="4">
+        <v>94539</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="H3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9648E4-D8BC-4082-BED6-0B9F506725CD}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col min="6" max="9" width="10.1796875" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="41.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="13">
+        <v>40909</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
5. ProfileDetailsPageTest is completed and ProfilePicturePersistenceTest is in progress.
</commit_message>
<xml_diff>
--- a/Excels/SimpleTherapy_Details.xlsx
+++ b/Excels/SimpleTherapy_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snehal-Vinayak\IdeaProjects\SimpleTherapy_Automation\SimpleTherapy_Web_Automation\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A353AF01-001D-4739-A126-F36DD0EB5EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0DBEF3-E97F-4429-B196-5E35827FA825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{4838E644-DBD1-4BD5-84C0-B33ABF6093BA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
   <si>
     <t>TitleHeading</t>
   </si>
@@ -235,6 +235,27 @@
   </si>
   <si>
     <t>California</t>
+  </si>
+  <si>
+    <t>1950 San Benito Dr</t>
+  </si>
+  <si>
+    <t>FirstName_Updated</t>
+  </si>
+  <si>
+    <t>Sagar1</t>
+  </si>
+  <si>
+    <t>LastName_Updated</t>
+  </si>
+  <si>
+    <t>City_Updated</t>
+  </si>
+  <si>
+    <t>Pangale1</t>
+  </si>
+  <si>
+    <t>Fremont1</t>
   </si>
 </sst>
 </file>
@@ -319,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -345,15 +366,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -914,41 +932,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9648E4-D8BC-4082-BED6-0B9F506725CD}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.1796875" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" customWidth="1"/>
-    <col min="4" max="4" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.81640625" customWidth="1"/>
-    <col min="6" max="9" width="10.1796875" customWidth="1"/>
-    <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="41.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="5.1796875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.1796875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.81640625" style="10" customWidth="1"/>
+    <col min="6" max="9" width="10.1796875" style="10" customWidth="1"/>
+    <col min="10" max="10" width="13" style="10" customWidth="1"/>
+    <col min="11" max="11" width="41.08984375" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="17.26953125" style="10" customWidth="1"/>
+    <col min="14" max="14" width="13.26953125" style="10" customWidth="1"/>
+    <col min="15" max="16384" width="8.7265625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>56</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>61</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -963,31 +984,40 @@
       <c r="J1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="7" t="s">
         <v>53</v>
       </c>
+      <c r="L1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="6" t="s">
         <v>59</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="13">
-        <v>40909</v>
+      <c r="F2" s="9">
+        <v>34700</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>63</v>
@@ -998,11 +1028,21 @@
       <c r="J2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="6" t="s">
         <v>60</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>